<commit_message>
introduced functionality for more flexible input reading
syntax-requirements remain
- input data numbered as index from 1 to N
- columns [Y,j,l]
- first index => y0 with j=l=0

To do:
- testing current version
- introduce user-defined output folder location + (sub-)folder generation
- automatic MDRM-Gauss LN approx, visualization (if requested), and ?? K-L divergence calculation or similar goodness of fit
</commit_message>
<xml_diff>
--- a/Ref02.xlsx
+++ b/Ref02.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
-    <t>X</t>
+    <t>CENTRAL</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
   </si>
 </sst>
 </file>
@@ -374,119 +383,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>37.019287582246</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>14.10361184023227</v>
+      </c>
+      <c r="D2">
+        <v>31.88389669424919</v>
+      </c>
+      <c r="E2">
+        <v>74.65580668962787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>37.4818568749157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>25.14925804642162</v>
+      </c>
+      <c r="D3">
+        <v>37.0349530383237</v>
+      </c>
+      <c r="E3">
+        <v>55.45427847716447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>37.1684358694446</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>42.39742708169723</v>
+      </c>
+      <c r="D4">
+        <v>42.39742708169723</v>
+      </c>
+      <c r="E4">
+        <v>42.39742708169723</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>36.8953307950117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>71.47494450253166</v>
+      </c>
+      <c r="D5">
+        <v>48.53636026722488</v>
+      </c>
+      <c r="E5">
+        <v>32.41484467042599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>36.5541479812791</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="C6">
+        <v>127.452587571939</v>
+      </c>
+      <c r="D6">
+        <v>56.37773326094273</v>
+      </c>
+      <c r="E6">
+        <v>24.07772285712328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>36.9282645442896</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>37.29389936567031</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>35.2994342966983</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>38.5512777265588</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>36.972987236855</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>35.9543185323955</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>41.0099828049857</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>39.3809394389494</v>
+        <v>42.39742708169723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>